<commit_message>
Changes to vlan id's and host profile identifiers
</commit_message>
<xml_diff>
--- a/spyglass/sample/SiteDesignSpec_v0.1.xlsx
+++ b/spyglass/sample/SiteDesignSpec_v0.1.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ericsson-my.sharepoint.com/personal/purnendu_ghosh_ericsson_com/Documents/AT&amp;T/LocalLab/temp/upstream/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eghopur\OneDrive - Ericsson AB\AT&amp;T\LocalLab\temp\upstream\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -16,7 +16,6 @@
     <sheet name="Site-Information" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="171027" concurrentCalc="0"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -67,27 +66,15 @@
     <t>iSCSI/Storage</t>
   </si>
   <si>
-    <t>vLAN 42</t>
-  </si>
-  <si>
     <t>PXE</t>
   </si>
   <si>
-    <t>vLAN 43</t>
-  </si>
-  <si>
     <t>Calico BGP peering addresses</t>
   </si>
   <si>
-    <t>vLAN 44</t>
-  </si>
-  <si>
     <t>Overlay</t>
   </si>
   <si>
-    <t>vLAN 45</t>
-  </si>
-  <si>
     <t>CNI Pod addresses</t>
   </si>
   <si>
@@ -100,9 +87,6 @@
     <t>VLAN</t>
   </si>
   <si>
-    <t>vlan 45</t>
-  </si>
-  <si>
     <t>POD</t>
   </si>
   <si>
@@ -116,9 +100,6 @@
   </si>
   <si>
     <t>Rack4</t>
-  </si>
-  <si>
-    <t>VLAN-41</t>
   </si>
   <si>
     <t>VLAN-49</t>
@@ -323,12 +304,6 @@
     <t>10.0.220.161</t>
   </si>
   <si>
-    <t>node-ctr-r720</t>
-  </si>
-  <si>
-    <t>node-cmp-r720</t>
-  </si>
-  <si>
     <t>SampleSiteName</t>
   </si>
   <si>
@@ -354,6 +329,30 @@
   </si>
   <si>
     <t>Sample Site Design File</t>
+  </si>
+  <si>
+    <t>vLAN 22</t>
+  </si>
+  <si>
+    <t>vLAN 23</t>
+  </si>
+  <si>
+    <t>vlan 24</t>
+  </si>
+  <si>
+    <t>VLAN-21</t>
+  </si>
+  <si>
+    <t>dp-r720</t>
+  </si>
+  <si>
+    <t>cp-r720</t>
+  </si>
+  <si>
+    <t>vLAN 24</t>
+  </si>
+  <si>
+    <t>vLAN 21</t>
   </si>
 </sst>
 </file>
@@ -477,7 +476,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -529,6 +528,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -657,7 +662,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -736,27 +741,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -766,6 +750,28 @@
     <xf numFmtId="0" fontId="2" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="15" fillId="9" borderId="7" xfId="3" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="15" fillId="9" borderId="8" xfId="3" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="6" xfId="3" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Hyperlink" xfId="4" builtinId="8"/>
@@ -1101,13 +1107,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:6" ht="29.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="40" t="s">
+      <c r="B1" s="48" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="41"/>
-      <c r="D1" s="41"/>
-      <c r="E1" s="41"/>
-      <c r="F1" s="42"/>
+      <c r="C1" s="49"/>
+      <c r="D1" s="49"/>
+      <c r="E1" s="49"/>
+      <c r="F1" s="50"/>
     </row>
     <row r="2" spans="2:6" ht="23.25" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
@@ -1137,16 +1143,16 @@
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B4" s="8" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="D4" s="10" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="E4" s="11" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="F4" s="11"/>
     </row>
@@ -1759,8 +1765,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:E62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1772,8 +1778,8 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="51" t="s">
-        <v>102</v>
+      <c r="A2" s="44" t="s">
+        <v>94</v>
       </c>
       <c r="B2" s="28"/>
     </row>
@@ -1793,388 +1799,388 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B4" s="22" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="C4" s="25" t="s">
-        <v>84</v>
-      </c>
-      <c r="D4" s="45" t="s">
-        <v>96</v>
-      </c>
-      <c r="E4" s="47" t="s">
-        <v>99</v>
+        <v>78</v>
+      </c>
+      <c r="D4" s="53" t="s">
+        <v>90</v>
+      </c>
+      <c r="E4" s="40" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B5" s="22" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="C5" s="25" t="s">
-        <v>85</v>
-      </c>
-      <c r="D5" s="45"/>
-      <c r="E5" s="47" t="s">
-        <v>99</v>
+        <v>79</v>
+      </c>
+      <c r="D5" s="53"/>
+      <c r="E5" s="40" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B6" s="22" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="C6" s="25" t="s">
-        <v>86</v>
-      </c>
-      <c r="D6" s="45"/>
-      <c r="E6" s="47" t="s">
-        <v>99</v>
+        <v>80</v>
+      </c>
+      <c r="D6" s="53"/>
+      <c r="E6" s="40" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B7" s="22" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="C7" s="25" t="s">
-        <v>87</v>
-      </c>
-      <c r="D7" s="45"/>
-      <c r="E7" s="47" t="s">
-        <v>99</v>
+        <v>81</v>
+      </c>
+      <c r="D7" s="53"/>
+      <c r="E7" s="40" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B8" s="22" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="C8" s="25" t="s">
-        <v>88</v>
-      </c>
-      <c r="D8" s="45"/>
-      <c r="E8" s="47" t="s">
-        <v>98</v>
+        <v>82</v>
+      </c>
+      <c r="D8" s="53"/>
+      <c r="E8" s="40" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B9" s="22" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="C9" s="25" t="s">
-        <v>89</v>
-      </c>
-      <c r="D9" s="45"/>
-      <c r="E9" s="47" t="s">
-        <v>98</v>
+        <v>83</v>
+      </c>
+      <c r="D9" s="53"/>
+      <c r="E9" s="40" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B10" s="22" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="C10" s="25" t="s">
-        <v>90</v>
-      </c>
-      <c r="D10" s="45" t="s">
-        <v>97</v>
-      </c>
-      <c r="E10" s="47" t="s">
-        <v>99</v>
+        <v>84</v>
+      </c>
+      <c r="D10" s="53" t="s">
+        <v>91</v>
+      </c>
+      <c r="E10" s="40" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B11" s="22" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="C11" s="25" t="s">
-        <v>91</v>
-      </c>
-      <c r="D11" s="45"/>
-      <c r="E11" s="47" t="s">
-        <v>99</v>
+        <v>85</v>
+      </c>
+      <c r="D11" s="53"/>
+      <c r="E11" s="40" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B12" s="22" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="C12" s="25" t="s">
-        <v>92</v>
-      </c>
-      <c r="D12" s="45"/>
-      <c r="E12" s="47" t="s">
-        <v>99</v>
+        <v>86</v>
+      </c>
+      <c r="D12" s="53"/>
+      <c r="E12" s="40" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B13" s="22" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="C13" s="25" t="s">
-        <v>93</v>
-      </c>
-      <c r="D13" s="45"/>
-      <c r="E13" s="47" t="s">
-        <v>99</v>
+        <v>87</v>
+      </c>
+      <c r="D13" s="53"/>
+      <c r="E13" s="40" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B14" s="22" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="C14" s="25" t="s">
-        <v>94</v>
-      </c>
-      <c r="D14" s="45"/>
-      <c r="E14" s="47" t="s">
-        <v>98</v>
+        <v>88</v>
+      </c>
+      <c r="D14" s="53"/>
+      <c r="E14" s="40" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B15" s="22" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="C15" s="25" t="s">
+        <v>89</v>
+      </c>
+      <c r="D15" s="53"/>
+      <c r="E15" s="40" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="44" t="s">
         <v>95</v>
       </c>
-      <c r="D15" s="45"/>
-      <c r="E15" s="47" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="51" t="s">
-        <v>103</v>
-      </c>
     </row>
     <row r="18" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A18" s="52" t="s">
+      <c r="A18" s="45" t="s">
         <v>11</v>
       </c>
-      <c r="B18" s="53" t="s">
-        <v>22</v>
+      <c r="B18" s="46" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="29" t="s">
         <v>12</v>
       </c>
-      <c r="B19" s="29" t="s">
-        <v>13</v>
+      <c r="B19" s="30" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="29" t="s">
-        <v>14</v>
-      </c>
-      <c r="B20" s="29" t="s">
-        <v>15</v>
+        <v>13</v>
+      </c>
+      <c r="B20" s="30" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="29" t="s">
-        <v>16</v>
-      </c>
-      <c r="B21" s="29" t="s">
-        <v>17</v>
+        <v>14</v>
+      </c>
+      <c r="B21" s="30" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="30" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B22" s="30" t="s">
-        <v>19</v>
+        <v>107</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="39" t="s">
-        <v>20</v>
-      </c>
-      <c r="B23" s="46" t="s">
-        <v>21</v>
+        <v>16</v>
+      </c>
+      <c r="B23" s="54" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="24" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" s="39"/>
-      <c r="B24" s="46"/>
+      <c r="B24" s="54"/>
     </row>
     <row r="25" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" s="39"/>
-      <c r="B25" s="46"/>
+      <c r="B25" s="54"/>
     </row>
     <row r="26" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" s="39"/>
-      <c r="B26" s="46"/>
+      <c r="B26" s="54"/>
     </row>
     <row r="27" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" s="39"/>
-      <c r="B27" s="46"/>
+      <c r="B27" s="54"/>
     </row>
     <row r="28" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" s="39"/>
-      <c r="B28" s="46"/>
+      <c r="B28" s="54"/>
     </row>
     <row r="29" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" s="39"/>
-      <c r="B29" s="46"/>
+      <c r="B29" s="54"/>
     </row>
     <row r="30" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30" s="39"/>
-      <c r="B30" s="46"/>
+      <c r="B30" s="54"/>
     </row>
     <row r="31" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32" s="48" t="s">
+      <c r="A32" s="41" t="s">
+        <v>19</v>
+      </c>
+      <c r="B32" s="42" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" s="35" t="s">
+        <v>102</v>
+      </c>
+      <c r="B33" s="29" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" s="35" t="s">
+        <v>108</v>
+      </c>
+      <c r="B34" s="29" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" s="33"/>
+      <c r="B35" s="29" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" s="33"/>
+      <c r="B36" s="29" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37" s="33"/>
+      <c r="B37" s="29" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="33"/>
+      <c r="B38" s="29"/>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39" s="35" t="s">
+        <v>101</v>
+      </c>
+      <c r="B39" s="30" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40" s="35" t="s">
+        <v>103</v>
+      </c>
+      <c r="B40" s="29" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A42" s="43" t="s">
+        <v>19</v>
+      </c>
+      <c r="B42" s="43" t="s">
+        <v>21</v>
+      </c>
+      <c r="C42" s="43" t="s">
+        <v>22</v>
+      </c>
+      <c r="D42" s="43" t="s">
         <v>23</v>
       </c>
-      <c r="B32" s="49" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" s="29" t="s">
-        <v>13</v>
-      </c>
-      <c r="B33" s="29" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" s="29" t="s">
-        <v>15</v>
-      </c>
-      <c r="B34" s="29" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35" s="29"/>
-      <c r="B35" s="29" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36" s="29"/>
-      <c r="B36" s="29" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37" s="29"/>
-      <c r="B37" s="29" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="29"/>
-      <c r="B38" s="29"/>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A39" s="29" t="s">
-        <v>17</v>
-      </c>
-      <c r="B39" s="30" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A40" s="30" t="s">
+      <c r="E42" s="43" t="s">
         <v>24</v>
       </c>
-      <c r="B40" s="29" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A42" s="50" t="s">
-        <v>23</v>
-      </c>
-      <c r="B42" s="50" t="s">
-        <v>26</v>
-      </c>
-      <c r="C42" s="50" t="s">
-        <v>27</v>
-      </c>
-      <c r="D42" s="50" t="s">
-        <v>28</v>
-      </c>
-      <c r="E42" s="50" t="s">
-        <v>29</v>
-      </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A43" s="33" t="s">
-        <v>30</v>
-      </c>
-      <c r="B43" s="43" t="s">
-        <v>74</v>
-      </c>
-      <c r="C43" s="44"/>
-      <c r="D43" s="44"/>
-      <c r="E43" s="44"/>
+      <c r="A43" s="47" t="s">
+        <v>104</v>
+      </c>
+      <c r="B43" s="51" t="s">
+        <v>68</v>
+      </c>
+      <c r="C43" s="52"/>
+      <c r="D43" s="52"/>
+      <c r="E43" s="52"/>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="33" t="s">
-        <v>31</v>
-      </c>
-      <c r="B44" s="43" t="s">
-        <v>75</v>
-      </c>
-      <c r="C44" s="44"/>
-      <c r="D44" s="44"/>
-      <c r="E44" s="44"/>
+        <v>25</v>
+      </c>
+      <c r="B44" s="51" t="s">
+        <v>69</v>
+      </c>
+      <c r="C44" s="52"/>
+      <c r="D44" s="52"/>
+      <c r="E44" s="52"/>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="33" t="s">
-        <v>32</v>
-      </c>
-      <c r="B45" s="43" t="s">
-        <v>76</v>
-      </c>
-      <c r="C45" s="44"/>
-      <c r="D45" s="44"/>
-      <c r="E45" s="44"/>
+        <v>26</v>
+      </c>
+      <c r="B45" s="51" t="s">
+        <v>70</v>
+      </c>
+      <c r="C45" s="52"/>
+      <c r="D45" s="52"/>
+      <c r="E45" s="52"/>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="34" t="s">
-        <v>33</v>
-      </c>
-      <c r="B46" s="43" t="s">
-        <v>77</v>
-      </c>
-      <c r="C46" s="44"/>
-      <c r="D46" s="44"/>
-      <c r="E46" s="44"/>
+        <v>27</v>
+      </c>
+      <c r="B46" s="51" t="s">
+        <v>71</v>
+      </c>
+      <c r="C46" s="52"/>
+      <c r="D46" s="52"/>
+      <c r="E46" s="52"/>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="33" t="s">
-        <v>34</v>
-      </c>
-      <c r="B47" s="43" t="s">
-        <v>82</v>
-      </c>
-      <c r="C47" s="44"/>
-      <c r="D47" s="44"/>
-      <c r="E47" s="44"/>
+        <v>28</v>
+      </c>
+      <c r="B47" s="51" t="s">
+        <v>76</v>
+      </c>
+      <c r="C47" s="52"/>
+      <c r="D47" s="52"/>
+      <c r="E47" s="52"/>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="35" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="B48" s="35" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="C48" s="35" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="D48" s="35" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="E48" s="35" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" s="27" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
     </row>
     <row r="50" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
@@ -2183,91 +2189,91 @@
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" s="36" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="B51" s="37" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" s="32" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="B52" s="31" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" s="32" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="B53" s="32" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" s="32" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="B54" s="37" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" s="32" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="B55" s="22" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
     </row>
     <row r="56" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A56" s="32" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="B56" s="38" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
     </row>
     <row r="57" spans="1:2" hidden="1" x14ac:dyDescent="0.25"/>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" s="32" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="B58" s="22" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" s="32" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="B59" s="22" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" s="32" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="B60" s="22" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" s="32" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="B61" s="22" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" s="32" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="B62" s="22" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
     </row>
   </sheetData>

</xml_diff>